<commit_message>
Retrofit Impl gestartet rest: token, alle kraftwerke
</commit_message>
<xml_diff>
--- a/Stundenliste.xlsx
+++ b/Stundenliste.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Stundenliste</t>
   </si>
@@ -44,15 +44,9 @@
     <t>Testprojekt erstellen</t>
   </si>
   <si>
-    <t>Beispiel apk mit Resty (login, alle Kraftwerke anzeigen)</t>
-  </si>
-  <si>
     <t>Exposé 1. Entwurf</t>
   </si>
   <si>
-    <t>latex installieren und Templet konfigurieren</t>
-  </si>
-  <si>
     <t>Exposé State of the Art</t>
   </si>
   <si>
@@ -63,6 +57,18 @@
   </si>
   <si>
     <t>Exposé fertig gestellt</t>
+  </si>
+  <si>
+    <t>Authentifizieren, alle Kraftwerke auslesen</t>
+  </si>
+  <si>
+    <t>Beispiel apk mit Resty (Login, alle Kraftwerke anzeigen)</t>
+  </si>
+  <si>
+    <t>Latex installieren und Templet konfigurieren</t>
+  </si>
+  <si>
+    <t>Retrofit eingelesen</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +447,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="2">
         <f>SUM(C3:C151)</f>
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -487,7 +493,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>6</v>
@@ -495,7 +501,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -503,7 +509,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>4</v>
@@ -511,7 +517,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -519,7 +525,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C12">
         <v>2.5</v>
@@ -530,7 +536,7 @@
         <v>42134</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -541,10 +547,32 @@
         <v>42136</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>42137</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>42138</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create grob fertig, ohne datepicker
</commit_message>
<xml_diff>
--- a/Stundenliste.xlsx
+++ b/Stundenliste.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Stundenliste</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>Retrofit eingelesen</t>
+  </si>
+  <si>
+    <t>Detail Overview</t>
+  </si>
+  <si>
+    <t>Evulution in Detail, BugFixes</t>
+  </si>
+  <si>
+    <t>create PowerPlant</t>
+  </si>
+  <si>
+    <t>create fertig gestellt, Design</t>
   </si>
 </sst>
 </file>
@@ -425,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +459,7 @@
       <c r="B2" s="1"/>
       <c r="C2" s="2">
         <f>SUM(C3:C151)</f>
-        <v>37</v>
+        <v>59.5</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -480,7 +492,7 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -550,7 +562,7 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -572,7 +584,51 @@
         <v>11</v>
       </c>
       <c r="C16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>42139</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>42141</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>42149</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
         <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>42151</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>